<commit_message>
Added perennial support & plant-json script Still may require some parameter tweaking
</commit_message>
<xml_diff>
--- a/Design docs/plant properties.xlsx
+++ b/Design docs/plant properties.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10870" uniqueCount="2465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10882" uniqueCount="2477">
   <si>
     <t>name_s</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -7512,6 +7512,132 @@
   </si>
   <si>
     <t>Bentgrass</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>isTree</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>isTree</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ormant height decrease</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ormant root length decrease</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>efault dormancy</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if this is true, give the plant the default values for decrease.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ormant stem</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ormant root</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ormant storage</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dormant fruits</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biomass object</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -7544,7 +7670,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7581,6 +7707,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -7591,7 +7723,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -7610,8 +7742,11 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -7645,13 +7780,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="6" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="20% - 강조색1" xfId="1" builtinId="30"/>
     <cellStyle name="20% - 강조색2" xfId="2" builtinId="34"/>
     <cellStyle name="20% - 강조색3" xfId="3" builtinId="38"/>
     <cellStyle name="20% - 강조색5" xfId="4" builtinId="46"/>
     <cellStyle name="20% - 강조색6" xfId="5" builtinId="50"/>
+    <cellStyle name="40% - 강조색2" xfId="6" builtinId="35"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7951,10 +8093,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN8"/>
+  <dimension ref="A1:AV8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7962,697 +8104,760 @@
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" t="s">
+        <v>2465</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>85</v>
       </c>
-      <c r="L1">
+      <c r="M1">
         <v>0.06</v>
       </c>
-      <c r="M1">
+      <c r="N1">
         <v>0.01</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="O1" s="8"/>
-      <c r="Q1" s="1">
+      <c r="P1" s="8"/>
+      <c r="R1" s="1">
         <v>7</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="1">
+      <c r="T1" s="1">
         <v>0.1</v>
       </c>
-      <c r="T1" s="1">
+      <c r="U1" s="1">
         <v>12</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AP1" t="s">
+        <v>2471</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>2476</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="8" t="s">
+        <v>2466</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>84</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>46</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>47</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="T2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="U2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="X2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AF2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AG2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AH2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AM2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AN2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AO2" s="11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AP2" s="12" t="s">
+        <v>2470</v>
+      </c>
+      <c r="AQ2" s="12" t="s">
+        <v>2468</v>
+      </c>
+      <c r="AR2" s="12" t="s">
+        <v>2469</v>
+      </c>
+      <c r="AS2" s="12" t="s">
+        <v>2472</v>
+      </c>
+      <c r="AT2" s="12" t="s">
+        <v>2473</v>
+      </c>
+      <c r="AU2" s="12" t="s">
+        <v>2474</v>
+      </c>
+      <c r="AV2" s="12" t="s">
+        <v>2475</v>
+      </c>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>800</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1093</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>1686</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>1800</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>5</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>2</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>1000</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>304</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>0.06</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>0.01</v>
       </c>
-      <c r="N3" t="b">
-        <v>0</v>
-      </c>
-      <c r="O3">
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3">
         <v>18</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>24</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>7</v>
       </c>
-      <c r="R3" t="b">
-        <v>1</v>
-      </c>
-      <c r="S3">
+      <c r="S3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T3">
         <v>0.1</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>12</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <f>15.55/2</f>
         <v>7.7750000000000004</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>23.55</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>0.6</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>0.4</v>
       </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
       <c r="Z3">
         <v>0</v>
       </c>
       <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
         <v>0.6</v>
       </c>
-      <c r="AB3">
+      <c r="AC3">
         <v>0.2</v>
       </c>
-      <c r="AC3">
-        <v>0</v>
-      </c>
       <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
         <v>0.2</v>
-      </c>
-      <c r="AE3">
-        <v>0.1</v>
       </c>
       <c r="AF3">
         <v>0.1</v>
       </c>
       <c r="AG3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
         <v>0.8</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <v>5</v>
       </c>
-      <c r="AJ3">
+      <c r="AK3">
         <v>12</v>
       </c>
-      <c r="AK3">
+      <c r="AL3">
         <v>7</v>
       </c>
-      <c r="AL3">
+      <c r="AM3">
         <v>0.05</v>
       </c>
-      <c r="AM3">
+      <c r="AN3">
         <v>0.5</v>
       </c>
-      <c r="AN3">
+      <c r="AO3">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AP3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>82</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>6</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>800</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1093</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>1686</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1800</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>5</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>2</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>610</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>304</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>0.06</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>0.01</v>
       </c>
-      <c r="N4" t="b">
-        <v>0</v>
-      </c>
-      <c r="O4">
+      <c r="O4" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4">
         <v>18</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>24</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>7</v>
       </c>
-      <c r="R4" t="b">
-        <v>1</v>
-      </c>
-      <c r="S4">
+      <c r="S4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4">
         <v>0.1</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>12</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <f>15.55/2</f>
         <v>7.7750000000000004</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>23.55</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>0.6</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>0.4</v>
       </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
       <c r="Z4">
         <v>0</v>
       </c>
       <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
         <v>0.6</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>0.2</v>
       </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
       <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
         <v>0.2</v>
-      </c>
-      <c r="AE4">
-        <v>0.1</v>
       </c>
       <c r="AF4">
         <v>0.1</v>
       </c>
       <c r="AG4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
         <v>0.8</v>
       </c>
-      <c r="AI4">
+      <c r="AJ4">
         <v>5</v>
       </c>
-      <c r="AJ4">
+      <c r="AK4">
         <v>12</v>
       </c>
-      <c r="AK4">
+      <c r="AL4">
         <v>7</v>
       </c>
-      <c r="AL4">
+      <c r="AM4">
         <v>0.05</v>
       </c>
-      <c r="AM4">
+      <c r="AN4">
         <v>0.5</v>
       </c>
-      <c r="AN4">
+      <c r="AO4">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AP4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>83</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>6</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>800</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1093</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>1686</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>1800</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>5</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
       <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
         <v>450</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>680</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>0.1</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>0.01</v>
       </c>
-      <c r="N5" t="b">
-        <v>1</v>
-      </c>
-      <c r="O5">
+      <c r="O5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5">
         <v>18</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>24</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>7</v>
       </c>
-      <c r="R5" t="b">
-        <v>1</v>
-      </c>
-      <c r="S5">
+      <c r="S5" t="b">
         <v>1</v>
       </c>
       <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
         <v>12</v>
       </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
       <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
         <v>12.5</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>0.6</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>0.4</v>
       </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
       <c r="Z5">
         <v>0</v>
       </c>
       <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
         <v>0.6</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <v>0.2</v>
       </c>
-      <c r="AC5">
-        <v>0</v>
-      </c>
       <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
         <v>0.2</v>
-      </c>
-      <c r="AE5">
-        <v>0.1</v>
       </c>
       <c r="AF5">
         <v>0.1</v>
       </c>
       <c r="AG5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
         <v>0.8</v>
       </c>
-      <c r="AI5">
+      <c r="AJ5">
         <v>10</v>
       </c>
-      <c r="AJ5">
+      <c r="AK5">
         <v>20</v>
       </c>
-      <c r="AK5">
+      <c r="AL5">
         <v>6</v>
       </c>
-      <c r="AL5">
+      <c r="AM5">
         <v>0.01</v>
       </c>
-      <c r="AM5">
-        <v>1</v>
-      </c>
       <c r="AN5">
+        <v>1</v>
+      </c>
+      <c r="AO5">
         <v>120</v>
       </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AP5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2462</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <v>3</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>800</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>1093</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>1686</v>
       </c>
-      <c r="G6">
-        <v>1800</v>
-      </c>
       <c r="H6">
+        <v>2600</v>
+      </c>
+      <c r="I6">
         <v>5</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>2</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>610</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>300</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>0.06</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>0.01</v>
       </c>
-      <c r="N6" t="b">
-        <v>1</v>
-      </c>
-      <c r="O6">
-        <v>18</v>
-      </c>
-      <c r="P6">
-        <v>24</v>
-      </c>
-      <c r="Q6">
-        <v>7</v>
-      </c>
-      <c r="R6" t="b">
-        <v>1</v>
-      </c>
-      <c r="S6">
-        <v>1</v>
-      </c>
-      <c r="T6">
-        <v>12</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
+      <c r="O6" t="b">
+        <v>1</v>
       </c>
       <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
         <v>15.5</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>0.6</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>0.4</v>
       </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
       <c r="Z6">
         <v>0</v>
       </c>
       <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
         <v>0.6</v>
       </c>
-      <c r="AB6">
+      <c r="AC6">
         <v>0.2</v>
       </c>
-      <c r="AC6">
-        <v>0</v>
-      </c>
       <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
         <v>0.2</v>
-      </c>
-      <c r="AE6">
-        <v>0.1</v>
       </c>
       <c r="AF6">
         <v>0.1</v>
       </c>
       <c r="AG6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
         <v>0.8</v>
       </c>
-      <c r="AI6">
+      <c r="AJ6">
         <v>10</v>
       </c>
-      <c r="AJ6">
+      <c r="AK6">
         <v>15</v>
       </c>
-      <c r="AK6">
+      <c r="AL6">
         <v>10</v>
       </c>
-      <c r="AL6">
+      <c r="AM6">
         <v>0.01</v>
       </c>
-      <c r="AM6">
-        <v>1</v>
-      </c>
       <c r="AN6">
+        <v>1</v>
+      </c>
+      <c r="AO6">
         <v>120</v>
       </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AP6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <v>0.998</v>
+      </c>
+      <c r="AR6">
+        <v>0.998</v>
+      </c>
+      <c r="AS6">
+        <v>0.995</v>
+      </c>
+      <c r="AT6">
+        <v>0.998</v>
+      </c>
+      <c r="AU6">
+        <v>0.995</v>
+      </c>
+      <c r="AV6">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2463</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2464</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8661,10 +8866,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8684,206 +8889,211 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>2467</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>